<commit_message>
Codigo de la pagina de la fac
</commit_message>
<xml_diff>
--- a/Excel/Septimo.xlsx
+++ b/Excel/Septimo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salvador\Documents\Generador de horarios\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ECDC47-F982-43E1-B938-6161F88E6255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD84D676-06D7-4EFA-B340-24B26924C57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6855" yWindow="2535" windowWidth="11415" windowHeight="11235" xr2:uid="{CCF8E56F-843D-445B-8045-8675589136B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="118">
   <si>
     <t>Clave</t>
   </si>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81580787-90D7-4675-BC96-0DEE297F141B}">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="H175" sqref="H175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +899,7 @@
       <c r="G2" s="7">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -913,9 +913,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -939,7 +937,7 @@
       <c r="G4" s="7">
         <v>38</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -953,9 +951,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="162" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -979,7 +975,7 @@
       <c r="G6" s="7">
         <v>40</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -993,9 +989,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="144.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -1037,9 +1031,7 @@
         <v>19</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -1063,7 +1055,7 @@
       <c r="G10" s="7">
         <v>45</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1077,9 +1069,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
@@ -1123,9 +1113,7 @@
         <v>28</v>
       </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
@@ -1169,9 +1157,7 @@
         <v>32</v>
       </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -1215,9 +1201,7 @@
         <v>31</v>
       </c>
       <c r="G17" s="8"/>
-      <c r="H17" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
@@ -1261,9 +1245,7 @@
         <v>38</v>
       </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" ht="144.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
@@ -1307,9 +1289,7 @@
         <v>31</v>
       </c>
       <c r="G21" s="8"/>
-      <c r="H21" s="6" t="s">
-        <v>112</v>
-      </c>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
@@ -1347,9 +1327,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
@@ -1387,9 +1365,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
@@ -1427,9 +1403,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1467,9 +1441,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
@@ -1507,9 +1479,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
@@ -1547,9 +1517,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
@@ -1587,9 +1555,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
@@ -1627,9 +1593,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
@@ -1667,9 +1631,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
@@ -1707,9 +1669,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
@@ -1747,9 +1707,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
@@ -1787,9 +1745,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
@@ -1827,9 +1783,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="6" t="s">
-        <v>114</v>
-      </c>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
@@ -1867,9 +1821,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
-      <c r="H49" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
@@ -1907,9 +1859,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H51" s="6"/>
     </row>
     <row r="52" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
@@ -1947,9 +1897,7 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-      <c r="H53" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
@@ -1987,9 +1935,7 @@
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
-      <c r="H55" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
@@ -2027,9 +1973,7 @@
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H57" s="6"/>
     </row>
     <row r="58" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
@@ -2067,9 +2011,7 @@
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H59" s="6"/>
     </row>
     <row r="60" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
@@ -2107,9 +2049,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
-      <c r="H61" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
@@ -2137,7 +2077,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="4" t="s">
@@ -2147,9 +2087,7 @@
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H63" s="6"/>
     </row>
     <row r="64" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
@@ -2177,7 +2115,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="C65" s="4" t="s">
@@ -2187,9 +2125,7 @@
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
       <c r="G65" s="8"/>
-      <c r="H65" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
@@ -2217,7 +2153,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="4" t="s">
@@ -2227,9 +2163,7 @@
       <c r="E67" s="8"/>
       <c r="F67" s="8"/>
       <c r="G67" s="8"/>
-      <c r="H67" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
@@ -2257,7 +2191,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="8"/>
       <c r="C69" s="4" t="s">
@@ -2267,9 +2201,7 @@
       <c r="E69" s="8"/>
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
-      <c r="H69" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H69" s="6"/>
     </row>
     <row r="70" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
@@ -2297,7 +2229,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="4" t="s">
@@ -2307,9 +2239,7 @@
       <c r="E71" s="8"/>
       <c r="F71" s="8"/>
       <c r="G71" s="8"/>
-      <c r="H71" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H71" s="6"/>
     </row>
     <row r="72" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
@@ -2337,7 +2267,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="8"/>
       <c r="C73" s="4" t="s">
@@ -2347,9 +2277,7 @@
       <c r="E73" s="8"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
-      <c r="H73" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
@@ -2377,7 +2305,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="8"/>
       <c r="B75" s="8"/>
       <c r="C75" s="4" t="s">
@@ -2387,9 +2315,7 @@
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
-      <c r="H75" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H75" s="6"/>
     </row>
     <row r="76" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
@@ -2417,7 +2343,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="4" t="s">
@@ -2427,9 +2353,7 @@
       <c r="E77" s="8"/>
       <c r="F77" s="8"/>
       <c r="G77" s="8"/>
-      <c r="H77" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
@@ -2457,7 +2381,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="C79" s="4" t="s">
@@ -2467,9 +2391,7 @@
       <c r="E79" s="8"/>
       <c r="F79" s="8"/>
       <c r="G79" s="8"/>
-      <c r="H79" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
@@ -2497,7 +2419,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="8"/>
       <c r="B81" s="8"/>
       <c r="C81" s="4" t="s">
@@ -2507,9 +2429,7 @@
       <c r="E81" s="8"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
-      <c r="H81" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H81" s="6"/>
     </row>
     <row r="82" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
@@ -2537,7 +2457,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="8"/>
       <c r="B83" s="8"/>
       <c r="C83" s="4" t="s">
@@ -2547,9 +2467,7 @@
       <c r="E83" s="8"/>
       <c r="F83" s="8"/>
       <c r="G83" s="8"/>
-      <c r="H83" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H83" s="6"/>
     </row>
     <row r="84" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
@@ -2577,7 +2495,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="8"/>
       <c r="B85" s="8"/>
       <c r="C85" s="4" t="s">
@@ -2587,9 +2505,7 @@
       <c r="E85" s="8"/>
       <c r="F85" s="8"/>
       <c r="G85" s="8"/>
-      <c r="H85" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H85" s="6"/>
     </row>
     <row r="86" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
@@ -2617,7 +2533,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="8"/>
       <c r="B87" s="8"/>
       <c r="C87" s="4" t="s">
@@ -2627,9 +2543,7 @@
       <c r="E87" s="8"/>
       <c r="F87" s="8"/>
       <c r="G87" s="8"/>
-      <c r="H87" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H87" s="6"/>
     </row>
     <row r="88" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
@@ -2657,7 +2571,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="8"/>
       <c r="C89" s="4" t="s">
@@ -2667,9 +2581,7 @@
       <c r="E89" s="8"/>
       <c r="F89" s="8"/>
       <c r="G89" s="8"/>
-      <c r="H89" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H89" s="6"/>
     </row>
     <row r="90" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
@@ -2697,7 +2609,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="4" t="s">
@@ -2707,9 +2619,7 @@
       <c r="E91" s="8"/>
       <c r="F91" s="8"/>
       <c r="G91" s="8"/>
-      <c r="H91" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H91" s="6"/>
     </row>
     <row r="92" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
@@ -2737,7 +2647,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="8"/>
       <c r="B93" s="8"/>
       <c r="C93" s="4" t="s">
@@ -2747,9 +2657,7 @@
       <c r="E93" s="8"/>
       <c r="F93" s="8"/>
       <c r="G93" s="8"/>
-      <c r="H93" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H93" s="6"/>
     </row>
     <row r="94" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
@@ -2777,7 +2685,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="4" t="s">
@@ -2787,9 +2695,7 @@
       <c r="E95" s="8"/>
       <c r="F95" s="8"/>
       <c r="G95" s="8"/>
-      <c r="H95" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H95" s="6"/>
     </row>
     <row r="96" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
@@ -2817,7 +2723,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="8"/>
       <c r="B97" s="8"/>
       <c r="C97" s="4" t="s">
@@ -2827,9 +2733,7 @@
       <c r="E97" s="8"/>
       <c r="F97" s="8"/>
       <c r="G97" s="8"/>
-      <c r="H97" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H97" s="6"/>
     </row>
     <row r="98" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
@@ -2857,7 +2761,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="8"/>
       <c r="B99" s="8"/>
       <c r="C99" s="4" t="s">
@@ -2867,9 +2771,7 @@
       <c r="E99" s="8"/>
       <c r="F99" s="8"/>
       <c r="G99" s="8"/>
-      <c r="H99" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H99" s="6"/>
     </row>
     <row r="100" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
@@ -2897,7 +2799,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="8"/>
       <c r="B101" s="8"/>
       <c r="C101" s="4" t="s">
@@ -2907,9 +2809,7 @@
       <c r="E101" s="8"/>
       <c r="F101" s="8"/>
       <c r="G101" s="8"/>
-      <c r="H101" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
@@ -2937,7 +2837,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="8"/>
       <c r="B103" s="8"/>
       <c r="C103" s="4" t="s">
@@ -2947,9 +2847,7 @@
       <c r="E103" s="8"/>
       <c r="F103" s="8"/>
       <c r="G103" s="8"/>
-      <c r="H103" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H103" s="6"/>
     </row>
     <row r="104" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
@@ -2977,7 +2875,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="8"/>
       <c r="B105" s="8"/>
       <c r="C105" s="4" t="s">
@@ -2987,9 +2885,7 @@
       <c r="E105" s="8"/>
       <c r="F105" s="8"/>
       <c r="G105" s="8"/>
-      <c r="H105" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H105" s="6"/>
     </row>
     <row r="106" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
@@ -3017,7 +2913,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="8"/>
       <c r="B107" s="8"/>
       <c r="C107" s="4" t="s">
@@ -3027,9 +2923,7 @@
       <c r="E107" s="8"/>
       <c r="F107" s="8"/>
       <c r="G107" s="8"/>
-      <c r="H107" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H107" s="6"/>
     </row>
     <row r="108" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
@@ -3057,7 +2951,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="C109" s="4" t="s">
@@ -3067,9 +2961,7 @@
       <c r="E109" s="8"/>
       <c r="F109" s="8"/>
       <c r="G109" s="8"/>
-      <c r="H109" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H109" s="6"/>
     </row>
     <row r="110" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
@@ -3097,7 +2989,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="8"/>
       <c r="B111" s="8"/>
       <c r="C111" s="4" t="s">
@@ -3107,9 +2999,7 @@
       <c r="E111" s="8"/>
       <c r="F111" s="8"/>
       <c r="G111" s="8"/>
-      <c r="H111" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H111" s="6"/>
     </row>
     <row r="112" spans="1:8" ht="162" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
@@ -3137,7 +3027,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="8"/>
       <c r="B113" s="8"/>
       <c r="C113" s="4" t="s">
@@ -3147,9 +3037,7 @@
       <c r="E113" s="8"/>
       <c r="F113" s="8"/>
       <c r="G113" s="8"/>
-      <c r="H113" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H113" s="6"/>
     </row>
     <row r="114" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
@@ -3177,7 +3065,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="8"/>
       <c r="B115" s="8"/>
       <c r="C115" s="4" t="s">
@@ -3187,9 +3075,7 @@
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
       <c r="G115" s="8"/>
-      <c r="H115" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H115" s="6"/>
     </row>
     <row r="116" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
@@ -3217,7 +3103,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="8"/>
       <c r="B117" s="8"/>
       <c r="C117" s="4" t="s">
@@ -3227,9 +3113,7 @@
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
       <c r="G117" s="8"/>
-      <c r="H117" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H117" s="6"/>
     </row>
     <row r="118" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
@@ -3257,7 +3141,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="8"/>
       <c r="B119" s="8"/>
       <c r="C119" s="4" t="s">
@@ -3267,9 +3151,7 @@
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
       <c r="G119" s="8"/>
-      <c r="H119" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H119" s="6"/>
     </row>
     <row r="120" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
@@ -3297,7 +3179,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="8"/>
       <c r="B121" s="8"/>
       <c r="C121" s="4" t="s">
@@ -3307,9 +3189,7 @@
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
       <c r="G121" s="8"/>
-      <c r="H121" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H121" s="6"/>
     </row>
     <row r="122" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
@@ -3337,7 +3217,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="8"/>
       <c r="B123" s="8"/>
       <c r="C123" s="4" t="s">
@@ -3347,9 +3227,7 @@
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
       <c r="G123" s="8"/>
-      <c r="H123" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H123" s="6"/>
     </row>
     <row r="124" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
@@ -3377,7 +3255,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="8"/>
       <c r="B125" s="8"/>
       <c r="C125" s="4" t="s">
@@ -3387,9 +3265,7 @@
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
       <c r="G125" s="8"/>
-      <c r="H125" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="H125" s="6"/>
     </row>
     <row r="126" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
@@ -3427,9 +3303,7 @@
       <c r="E127" s="8"/>
       <c r="F127" s="8"/>
       <c r="G127" s="8"/>
-      <c r="H127" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H127" s="6"/>
     </row>
     <row r="128" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
@@ -3467,9 +3341,7 @@
       <c r="E129" s="8"/>
       <c r="F129" s="8"/>
       <c r="G129" s="8"/>
-      <c r="H129" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H129" s="6"/>
     </row>
     <row r="130" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A130" s="7">
@@ -3507,9 +3379,7 @@
       <c r="E131" s="8"/>
       <c r="F131" s="8"/>
       <c r="G131" s="8"/>
-      <c r="H131" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H131" s="6"/>
     </row>
     <row r="132" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A132" s="7">
@@ -3547,9 +3417,7 @@
       <c r="E133" s="8"/>
       <c r="F133" s="8"/>
       <c r="G133" s="8"/>
-      <c r="H133" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H133" s="6"/>
     </row>
     <row r="134" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A134" s="7">
@@ -3587,9 +3455,7 @@
       <c r="E135" s="8"/>
       <c r="F135" s="8"/>
       <c r="G135" s="8"/>
-      <c r="H135" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H135" s="6"/>
     </row>
     <row r="136" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A136" s="7">
@@ -3627,9 +3493,7 @@
       <c r="E137" s="8"/>
       <c r="F137" s="8"/>
       <c r="G137" s="8"/>
-      <c r="H137" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H137" s="6"/>
     </row>
     <row r="138" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A138" s="7">
@@ -3667,9 +3531,7 @@
       <c r="E139" s="8"/>
       <c r="F139" s="8"/>
       <c r="G139" s="8"/>
-      <c r="H139" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H139" s="6"/>
     </row>
     <row r="140" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A140" s="7">
@@ -3707,9 +3569,7 @@
       <c r="E141" s="8"/>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
-      <c r="H141" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H141" s="6"/>
     </row>
     <row r="142" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A142" s="7">
@@ -3747,9 +3607,7 @@
       <c r="E143" s="8"/>
       <c r="F143" s="8"/>
       <c r="G143" s="8"/>
-      <c r="H143" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H143" s="6"/>
     </row>
     <row r="144" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A144" s="7">
@@ -3787,9 +3645,7 @@
       <c r="E145" s="8"/>
       <c r="F145" s="8"/>
       <c r="G145" s="8"/>
-      <c r="H145" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H145" s="6"/>
     </row>
     <row r="146" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A146" s="7">
@@ -3827,9 +3683,7 @@
       <c r="E147" s="8"/>
       <c r="F147" s="8"/>
       <c r="G147" s="8"/>
-      <c r="H147" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H147" s="6"/>
     </row>
     <row r="148" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A148" s="7">
@@ -3867,9 +3721,7 @@
       <c r="E149" s="8"/>
       <c r="F149" s="8"/>
       <c r="G149" s="8"/>
-      <c r="H149" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H149" s="6"/>
     </row>
     <row r="150" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A150" s="7">
@@ -3907,9 +3759,7 @@
       <c r="E151" s="8"/>
       <c r="F151" s="8"/>
       <c r="G151" s="8"/>
-      <c r="H151" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H151" s="6"/>
     </row>
     <row r="152" spans="1:8" ht="162" x14ac:dyDescent="0.25">
       <c r="A152" s="7">
@@ -3947,9 +3797,7 @@
       <c r="E153" s="8"/>
       <c r="F153" s="8"/>
       <c r="G153" s="8"/>
-      <c r="H153" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H153" s="6"/>
     </row>
     <row r="154" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A154" s="7">
@@ -3987,9 +3835,7 @@
       <c r="E155" s="8"/>
       <c r="F155" s="8"/>
       <c r="G155" s="8"/>
-      <c r="H155" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H155" s="6"/>
     </row>
     <row r="156" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A156" s="7">
@@ -4027,9 +3873,7 @@
       <c r="E157" s="8"/>
       <c r="F157" s="8"/>
       <c r="G157" s="8"/>
-      <c r="H157" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H157" s="6"/>
     </row>
     <row r="158" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A158" s="7">
@@ -4067,9 +3911,7 @@
       <c r="E159" s="8"/>
       <c r="F159" s="8"/>
       <c r="G159" s="8"/>
-      <c r="H159" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H159" s="6"/>
     </row>
     <row r="160" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A160" s="7">
@@ -4107,9 +3949,7 @@
       <c r="E161" s="8"/>
       <c r="F161" s="8"/>
       <c r="G161" s="8"/>
-      <c r="H161" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H161" s="6"/>
     </row>
     <row r="162" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A162" s="7">
@@ -4147,9 +3987,7 @@
       <c r="E163" s="8"/>
       <c r="F163" s="8"/>
       <c r="G163" s="8"/>
-      <c r="H163" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H163" s="6"/>
     </row>
     <row r="164" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A164" s="7">
@@ -4187,9 +4025,7 @@
       <c r="E165" s="8"/>
       <c r="F165" s="8"/>
       <c r="G165" s="8"/>
-      <c r="H165" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H165" s="6"/>
     </row>
     <row r="166" spans="1:8" ht="72" x14ac:dyDescent="0.25">
       <c r="A166" s="7">
@@ -4227,9 +4063,7 @@
       <c r="E167" s="8"/>
       <c r="F167" s="8"/>
       <c r="G167" s="8"/>
-      <c r="H167" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H167" s="6"/>
     </row>
     <row r="168" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A168" s="7">
@@ -4267,9 +4101,7 @@
       <c r="E169" s="8"/>
       <c r="F169" s="8"/>
       <c r="G169" s="8"/>
-      <c r="H169" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H169" s="6"/>
     </row>
     <row r="170" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A170" s="7">
@@ -4307,9 +4139,7 @@
       <c r="E171" s="8"/>
       <c r="F171" s="8"/>
       <c r="G171" s="8"/>
-      <c r="H171" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H171" s="6"/>
     </row>
     <row r="172" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A172" s="7">
@@ -4347,9 +4177,7 @@
       <c r="E173" s="8"/>
       <c r="F173" s="8"/>
       <c r="G173" s="8"/>
-      <c r="H173" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H173" s="6"/>
     </row>
     <row r="174" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A174" s="7">
@@ -4387,12 +4215,497 @@
       <c r="E175" s="8"/>
       <c r="F175" s="8"/>
       <c r="G175" s="8"/>
-      <c r="H175" s="6" t="s">
-        <v>117</v>
-      </c>
+      <c r="H175" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="505">
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="D174:D175"/>
+    <mergeCell ref="E174:E175"/>
+    <mergeCell ref="F174:F175"/>
+    <mergeCell ref="G174:G175"/>
+    <mergeCell ref="A172:A173"/>
+    <mergeCell ref="B172:B173"/>
+    <mergeCell ref="D172:D173"/>
+    <mergeCell ref="E172:E173"/>
+    <mergeCell ref="F172:F173"/>
+    <mergeCell ref="G172:G173"/>
+    <mergeCell ref="A170:A171"/>
+    <mergeCell ref="B170:B171"/>
+    <mergeCell ref="D170:D171"/>
+    <mergeCell ref="E170:E171"/>
+    <mergeCell ref="F170:F171"/>
+    <mergeCell ref="G170:G171"/>
+    <mergeCell ref="A168:A169"/>
+    <mergeCell ref="B168:B169"/>
+    <mergeCell ref="D168:D169"/>
+    <mergeCell ref="E168:E169"/>
+    <mergeCell ref="F168:F169"/>
+    <mergeCell ref="G168:G169"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="B166:B167"/>
+    <mergeCell ref="D166:D167"/>
+    <mergeCell ref="E166:E167"/>
+    <mergeCell ref="F166:F167"/>
+    <mergeCell ref="G166:G167"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="B164:B165"/>
+    <mergeCell ref="D164:D165"/>
+    <mergeCell ref="E164:E165"/>
+    <mergeCell ref="F164:F165"/>
+    <mergeCell ref="G164:G165"/>
+    <mergeCell ref="A162:A163"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="D162:D163"/>
+    <mergeCell ref="E162:E163"/>
+    <mergeCell ref="F162:F163"/>
+    <mergeCell ref="G162:G163"/>
+    <mergeCell ref="A160:A161"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="D160:D161"/>
+    <mergeCell ref="E160:E161"/>
+    <mergeCell ref="F160:F161"/>
+    <mergeCell ref="G160:G161"/>
+    <mergeCell ref="A158:A159"/>
+    <mergeCell ref="B158:B159"/>
+    <mergeCell ref="D158:D159"/>
+    <mergeCell ref="E158:E159"/>
+    <mergeCell ref="F158:F159"/>
+    <mergeCell ref="G158:G159"/>
+    <mergeCell ref="A156:A157"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="D156:D157"/>
+    <mergeCell ref="E156:E157"/>
+    <mergeCell ref="F156:F157"/>
+    <mergeCell ref="G156:G157"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="D154:D155"/>
+    <mergeCell ref="E154:E155"/>
+    <mergeCell ref="F154:F155"/>
+    <mergeCell ref="G154:G155"/>
+    <mergeCell ref="A152:A153"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="E152:E153"/>
+    <mergeCell ref="F152:F153"/>
+    <mergeCell ref="G152:G153"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="D150:D151"/>
+    <mergeCell ref="E150:E151"/>
+    <mergeCell ref="F150:F151"/>
+    <mergeCell ref="G150:G151"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="D148:D149"/>
+    <mergeCell ref="E148:E149"/>
+    <mergeCell ref="F148:F149"/>
+    <mergeCell ref="G148:G149"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="F146:F147"/>
+    <mergeCell ref="G146:G147"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="D144:D145"/>
+    <mergeCell ref="E144:E145"/>
+    <mergeCell ref="F144:F145"/>
+    <mergeCell ref="G144:G145"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="E142:E143"/>
+    <mergeCell ref="F142:F143"/>
+    <mergeCell ref="G142:G143"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="D140:D141"/>
+    <mergeCell ref="E140:E141"/>
+    <mergeCell ref="F140:F141"/>
+    <mergeCell ref="G140:G141"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="F138:F139"/>
+    <mergeCell ref="G138:G139"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="D136:D137"/>
+    <mergeCell ref="E136:E137"/>
+    <mergeCell ref="F136:F137"/>
+    <mergeCell ref="G136:G137"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="D134:D135"/>
+    <mergeCell ref="E134:E135"/>
+    <mergeCell ref="F134:F135"/>
+    <mergeCell ref="G134:G135"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:F133"/>
+    <mergeCell ref="G132:G133"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="D130:D131"/>
+    <mergeCell ref="E130:E131"/>
+    <mergeCell ref="F130:F131"/>
+    <mergeCell ref="G130:G131"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="E128:E129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="F126:F127"/>
+    <mergeCell ref="G126:G127"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="D122:D123"/>
+    <mergeCell ref="E122:E123"/>
+    <mergeCell ref="F122:F123"/>
+    <mergeCell ref="G122:G123"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="F120:F121"/>
+    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="E118:E119"/>
+    <mergeCell ref="F118:F119"/>
+    <mergeCell ref="G118:G119"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:F117"/>
+    <mergeCell ref="G116:G117"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="D114:D115"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="F114:F115"/>
+    <mergeCell ref="G114:G115"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="F112:F113"/>
+    <mergeCell ref="G112:G113"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="D110:D111"/>
+    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="F110:F111"/>
+    <mergeCell ref="G110:G111"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="F108:F109"/>
+    <mergeCell ref="G108:G109"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="G106:G107"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="D102:D103"/>
+    <mergeCell ref="E102:E103"/>
+    <mergeCell ref="F102:F103"/>
+    <mergeCell ref="G102:G103"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="D100:D101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="F100:F101"/>
+    <mergeCell ref="G100:G101"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="D98:D99"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="F98:F99"/>
+    <mergeCell ref="G98:G99"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="D96:D97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="F96:F97"/>
+    <mergeCell ref="G96:G97"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="D94:D95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="F94:F95"/>
+    <mergeCell ref="G94:G95"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="G92:G93"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="G88:G89"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="G84:G85"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="F80:F81"/>
+    <mergeCell ref="G80:G81"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="G72:G73"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
@@ -4411,493 +4724,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="G72:G73"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="G78:G79"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="G76:G77"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:F83"/>
-    <mergeCell ref="G82:G83"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="F80:F81"/>
-    <mergeCell ref="G80:G81"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="G84:G85"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="G90:G91"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="G88:G89"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="D94:D95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="F94:F95"/>
-    <mergeCell ref="G94:G95"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="D92:D93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="G92:G93"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="D98:D99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="F98:F99"/>
-    <mergeCell ref="G98:G99"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="D96:D97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="F96:F97"/>
-    <mergeCell ref="G96:G97"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="D102:D103"/>
-    <mergeCell ref="E102:E103"/>
-    <mergeCell ref="F102:F103"/>
-    <mergeCell ref="G102:G103"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="D100:D101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="F100:F101"/>
-    <mergeCell ref="G100:G101"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="G106:G107"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="G104:G105"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="D110:D111"/>
-    <mergeCell ref="E110:E111"/>
-    <mergeCell ref="F110:F111"/>
-    <mergeCell ref="G110:G111"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="E108:E109"/>
-    <mergeCell ref="F108:F109"/>
-    <mergeCell ref="G108:G109"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="D114:D115"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="F114:F115"/>
-    <mergeCell ref="G114:G115"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="D112:D113"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="F112:F113"/>
-    <mergeCell ref="G112:G113"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="D118:D119"/>
-    <mergeCell ref="E118:E119"/>
-    <mergeCell ref="F118:F119"/>
-    <mergeCell ref="G118:G119"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="B116:B117"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:F117"/>
-    <mergeCell ref="G116:G117"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="D122:D123"/>
-    <mergeCell ref="E122:E123"/>
-    <mergeCell ref="F122:F123"/>
-    <mergeCell ref="G122:G123"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="F120:F121"/>
-    <mergeCell ref="G120:G121"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="D126:D127"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="F126:F127"/>
-    <mergeCell ref="G126:G127"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="F124:F125"/>
-    <mergeCell ref="G124:G125"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="D130:D131"/>
-    <mergeCell ref="E130:E131"/>
-    <mergeCell ref="F130:F131"/>
-    <mergeCell ref="G130:G131"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="E128:E129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="D134:D135"/>
-    <mergeCell ref="E134:E135"/>
-    <mergeCell ref="F134:F135"/>
-    <mergeCell ref="G134:G135"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F132:F133"/>
-    <mergeCell ref="G132:G133"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="D138:D139"/>
-    <mergeCell ref="E138:E139"/>
-    <mergeCell ref="F138:F139"/>
-    <mergeCell ref="G138:G139"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="D136:D137"/>
-    <mergeCell ref="E136:E137"/>
-    <mergeCell ref="F136:F137"/>
-    <mergeCell ref="G136:G137"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="E142:E143"/>
-    <mergeCell ref="F142:F143"/>
-    <mergeCell ref="G142:G143"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="B140:B141"/>
-    <mergeCell ref="D140:D141"/>
-    <mergeCell ref="E140:E141"/>
-    <mergeCell ref="F140:F141"/>
-    <mergeCell ref="G140:G141"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="D146:D147"/>
-    <mergeCell ref="E146:E147"/>
-    <mergeCell ref="F146:F147"/>
-    <mergeCell ref="G146:G147"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="D144:D145"/>
-    <mergeCell ref="E144:E145"/>
-    <mergeCell ref="F144:F145"/>
-    <mergeCell ref="G144:G145"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="D150:D151"/>
-    <mergeCell ref="E150:E151"/>
-    <mergeCell ref="F150:F151"/>
-    <mergeCell ref="G150:G151"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="B148:B149"/>
-    <mergeCell ref="D148:D149"/>
-    <mergeCell ref="E148:E149"/>
-    <mergeCell ref="F148:F149"/>
-    <mergeCell ref="G148:G149"/>
-    <mergeCell ref="A154:A155"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="D154:D155"/>
-    <mergeCell ref="E154:E155"/>
-    <mergeCell ref="F154:F155"/>
-    <mergeCell ref="G154:G155"/>
-    <mergeCell ref="A152:A153"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="D152:D153"/>
-    <mergeCell ref="E152:E153"/>
-    <mergeCell ref="F152:F153"/>
-    <mergeCell ref="G152:G153"/>
-    <mergeCell ref="A158:A159"/>
-    <mergeCell ref="B158:B159"/>
-    <mergeCell ref="D158:D159"/>
-    <mergeCell ref="E158:E159"/>
-    <mergeCell ref="F158:F159"/>
-    <mergeCell ref="G158:G159"/>
-    <mergeCell ref="A156:A157"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="D156:D157"/>
-    <mergeCell ref="E156:E157"/>
-    <mergeCell ref="F156:F157"/>
-    <mergeCell ref="G156:G157"/>
-    <mergeCell ref="A162:A163"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="D162:D163"/>
-    <mergeCell ref="E162:E163"/>
-    <mergeCell ref="F162:F163"/>
-    <mergeCell ref="G162:G163"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="E160:E161"/>
-    <mergeCell ref="F160:F161"/>
-    <mergeCell ref="G160:G161"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="B166:B167"/>
-    <mergeCell ref="D166:D167"/>
-    <mergeCell ref="E166:E167"/>
-    <mergeCell ref="F166:F167"/>
-    <mergeCell ref="G166:G167"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="D164:D165"/>
-    <mergeCell ref="E164:E165"/>
-    <mergeCell ref="F164:F165"/>
-    <mergeCell ref="G164:G165"/>
-    <mergeCell ref="A170:A171"/>
-    <mergeCell ref="B170:B171"/>
-    <mergeCell ref="D170:D171"/>
-    <mergeCell ref="E170:E171"/>
-    <mergeCell ref="F170:F171"/>
-    <mergeCell ref="G170:G171"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="B168:B169"/>
-    <mergeCell ref="D168:D169"/>
-    <mergeCell ref="E168:E169"/>
-    <mergeCell ref="F168:F169"/>
-    <mergeCell ref="G168:G169"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="D174:D175"/>
-    <mergeCell ref="E174:E175"/>
-    <mergeCell ref="F174:F175"/>
-    <mergeCell ref="G174:G175"/>
-    <mergeCell ref="A172:A173"/>
-    <mergeCell ref="B172:B173"/>
-    <mergeCell ref="D172:D173"/>
-    <mergeCell ref="E172:E173"/>
-    <mergeCell ref="F172:F173"/>
-    <mergeCell ref="G172:G173"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>